<commit_message>
update by set filter to 4; change fnn's model construction
</commit_message>
<xml_diff>
--- a/A6worksheetV2.xlsx
+++ b/A6worksheetV2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpluskira/studyabroad/Rice/DataSci/A6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4452AB-F60C-BF48-8C92-52FC926CBDD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E66DD3-FD48-6A4E-9979-7A557BDCFD02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,13 +631,13 @@
         <v>5</v>
       </c>
       <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
         <v>623</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
@@ -655,13 +655,13 @@
         <v>6</v>
       </c>
       <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
         <v>620</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -680,14 +680,14 @@
       <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
         <v>620</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -705,13 +705,13 @@
         <v>8</v>
       </c>
       <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
         <v>624</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
       </c>
       <c r="I12" s="2">
         <v>0</v>
@@ -729,14 +729,14 @@
         <v>9</v>
       </c>
       <c r="F13" s="2">
-        <f>F9 + F10 + F11 + F12</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <f>H9 + H10 + H11 + H12</f>
         <v>2487</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -795,23 +795,23 @@
       <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="2">
-        <v>0.250502613590671</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="F16">
+        <v>0.74949738640932795</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>1</v>
       </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.250502613590671</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.40064308681672001</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0.62562763607149996</v>
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -821,22 +821,22 @@
       <c r="E17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <v>0.75070365902694003</v>
       </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" t="s">
         <v>39</v>
       </c>
     </row>
@@ -847,23 +847,23 @@
       <c r="E18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="2">
-        <v>0.75070365902694003</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
+      <c r="F18">
+        <v>0.249296340973059</v>
+      </c>
+      <c r="G18">
         <v>1</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>39</v>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0.249296340973059</v>
+      </c>
+      <c r="J18">
+        <v>0.39909880914064999</v>
+      </c>
+      <c r="K18">
+        <v>0.62411918663176902</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -873,22 +873,22 @@
       <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="2">
-        <v>0.75070365902694003</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="F19">
+        <v>0.74909529553679099</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" t="s">
         <v>39</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" t="s">
         <v>39</v>
       </c>
     </row>
@@ -983,16 +983,16 @@
         <v>5</v>
       </c>
       <c r="F28" s="2">
-        <v>250</v>
+        <v>126</v>
       </c>
       <c r="G28" s="2">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="H28" s="2">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="I28" s="2">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="J28" s="2">
         <f>SUM(F28:I28)</f>
@@ -1008,16 +1008,16 @@
         <v>6</v>
       </c>
       <c r="F29" s="2">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="G29" s="2">
-        <v>277</v>
+        <v>323</v>
       </c>
       <c r="H29" s="2">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="I29" s="2">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" ref="J29:J31" si="0">SUM(F29:I29)</f>
@@ -1035,16 +1035,16 @@
         <v>7</v>
       </c>
       <c r="F30" s="7">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="G30" s="2">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="H30" s="2">
-        <v>421</v>
+        <v>457</v>
       </c>
       <c r="I30" s="2">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" si="0"/>
@@ -1060,19 +1060,18 @@
         <v>8</v>
       </c>
       <c r="F31" s="2">
-        <v>206</v>
+        <v>96</v>
       </c>
       <c r="G31" s="2">
-        <v>47</v>
+        <v>135</v>
       </c>
       <c r="H31" s="2">
-        <v>107</v>
+        <v>166</v>
       </c>
       <c r="I31" s="2">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="0"/>
         <v>624</v>
       </c>
     </row>
@@ -1086,19 +1085,19 @@
       </c>
       <c r="F32" s="2">
         <f>SUM(F28:F31)</f>
-        <v>609</v>
+        <v>284</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" ref="G32:I32" si="1">SUM(G28:G31)</f>
-        <v>400</v>
+        <v>680</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" si="1"/>
-        <v>649</v>
+        <v>770</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" si="1"/>
-        <v>829</v>
+        <v>803</v>
       </c>
       <c r="J32" s="2">
         <f>J28 + J29 + J30 + J31</f>
@@ -1155,22 +1154,22 @@
         <v>5</v>
       </c>
       <c r="F35" s="2">
-        <v>0.70566948130277396</v>
+        <v>0.73663047848813801</v>
       </c>
       <c r="G35" s="2">
-        <v>0.40128410914927698</v>
+        <v>0.20224719101123501</v>
       </c>
       <c r="H35" s="2">
-        <v>0.80740343347639398</v>
+        <v>0.91523605150214504</v>
       </c>
       <c r="I35" s="2">
-        <v>0.41050903119868598</v>
+        <v>0.44366197183098499</v>
       </c>
       <c r="J35" s="2">
-        <v>0.40584415584415501</v>
+        <v>0.27783902976846703</v>
       </c>
       <c r="K35" s="2">
-        <v>0.40309577555627202</v>
+        <v>0.22694524495677201</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1181,22 +1180,22 @@
         <v>6</v>
       </c>
       <c r="F36" s="2">
-        <v>0.81262565339766701</v>
+        <v>0.73703256936067496</v>
       </c>
       <c r="G36" s="2">
-        <v>0.44677419354838699</v>
+        <v>0.52096774193548301</v>
       </c>
       <c r="H36" s="2">
-        <v>0.93411890733797498</v>
+        <v>0.80878414568826995</v>
       </c>
       <c r="I36" s="2">
-        <v>0.6925</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="J36" s="2">
-        <v>0.54313725490195996</v>
+        <v>0.49692307692307602</v>
       </c>
       <c r="K36" s="2">
-        <v>0.48090277777777701</v>
+        <v>0.511075949367088</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1207,22 +1206,22 @@
         <v>7</v>
       </c>
       <c r="F37" s="2">
-        <v>0.82830719742661796</v>
+        <v>0.80860474467229504</v>
       </c>
       <c r="G37" s="2">
-        <v>0.67903225806451595</v>
+        <v>0.73709677419354802</v>
       </c>
       <c r="H37" s="2">
-        <v>0.87787895018746598</v>
+        <v>0.83235136582753</v>
       </c>
       <c r="I37" s="2">
-        <v>0.64869029275808898</v>
+        <v>0.59350649350649298</v>
       </c>
       <c r="J37" s="2">
-        <v>0.66351457840819505</v>
+        <v>0.65755395683453199</v>
       </c>
       <c r="K37" s="2">
-        <v>0.672738894215404</v>
+        <v>0.70307692307692204</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1233,22 +1232,22 @@
         <v>8</v>
       </c>
       <c r="F38" s="2">
-        <v>0.62806594290309603</v>
+        <v>0.62887012464817005</v>
       </c>
       <c r="G38" s="2">
-        <v>0.42307692307692302</v>
+        <v>0.36378205128205099</v>
       </c>
       <c r="H38" s="2">
-        <v>0.69672571121846405</v>
+        <v>0.71765968867418095</v>
       </c>
       <c r="I38" s="2">
-        <v>0.318455971049457</v>
+        <v>0.30146082337317398</v>
       </c>
       <c r="J38" s="2">
-        <v>0.36338609772883601</v>
+        <v>0.32970225127087799</v>
       </c>
       <c r="K38" s="2">
-        <v>0.39699248120300701</v>
+        <v>0.34933825792551498</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1390,16 +1389,16 @@
         <v>5</v>
       </c>
       <c r="F53" s="2">
-        <v>177</v>
+        <v>270</v>
       </c>
       <c r="G53" s="2">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="H53" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I53" s="2">
-        <v>305</v>
+        <v>251</v>
       </c>
       <c r="J53" s="2">
         <f>SUM(F53:I53)</f>
@@ -1415,16 +1414,16 @@
         <v>6</v>
       </c>
       <c r="F54" s="2">
-        <v>48</v>
+        <v>130</v>
       </c>
       <c r="G54" s="2">
-        <v>320</v>
+        <v>197</v>
       </c>
       <c r="H54" s="2">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="I54" s="2">
-        <v>196</v>
+        <v>278</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" ref="J54:J56" si="2">SUM(F54:I54)</f>
@@ -1442,16 +1441,16 @@
         <v>7</v>
       </c>
       <c r="F55" s="7">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="G55" s="2">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="H55" s="2">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="I55" s="2">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" si="2"/>
@@ -1467,16 +1466,16 @@
         <v>8</v>
       </c>
       <c r="F56" s="2">
-        <v>167</v>
+        <v>242</v>
       </c>
       <c r="G56" s="2">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="H56" s="2">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="I56" s="2">
-        <v>272</v>
+        <v>302</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" si="2"/>
@@ -1493,19 +1492,19 @@
       </c>
       <c r="F57" s="2">
         <f>SUM(F53:F56)</f>
-        <v>434</v>
+        <v>727</v>
       </c>
       <c r="G57" s="2">
         <f t="shared" ref="G57:I57" si="3">SUM(G53:G56)</f>
-        <v>633</v>
+        <v>318</v>
       </c>
       <c r="H57" s="2">
         <f t="shared" si="3"/>
-        <v>512</v>
+        <v>428</v>
       </c>
       <c r="I57" s="2">
         <f t="shared" si="3"/>
-        <v>908</v>
+        <v>1014</v>
       </c>
       <c r="J57" s="2">
         <f>J53 + J54 + J55 + J56</f>
@@ -1562,22 +1561,22 @@
         <v>5</v>
       </c>
       <c r="F60" s="2">
-        <v>0.71733011660635304</v>
+        <v>0.67430639324487296</v>
       </c>
       <c r="G60" s="2">
-        <v>0.28410914927768799</v>
+        <v>0.43338683788121901</v>
       </c>
       <c r="H60" s="2">
-        <v>0.86212446351931304</v>
+        <v>0.75482832618025697</v>
       </c>
       <c r="I60" s="2">
-        <v>0.40783410138248799</v>
+        <v>0.371389270976616</v>
       </c>
       <c r="J60" s="2">
-        <v>0.334910122989593</v>
+        <v>0.4</v>
       </c>
       <c r="K60" s="2">
-        <v>0.30246069719753899</v>
+        <v>0.41938490214352198</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -1588,22 +1587,22 @@
         <v>6</v>
       </c>
       <c r="F61" s="2">
-        <v>0.75351829513470003</v>
+        <v>0.78126256533976601</v>
       </c>
       <c r="G61" s="2">
-        <v>0.51612903225806395</v>
+        <v>0.31774193548387097</v>
       </c>
       <c r="H61" s="2">
-        <v>0.83235136582753</v>
+        <v>0.93519014461703198</v>
       </c>
       <c r="I61" s="2">
-        <v>0.50552922590837202</v>
+        <v>0.61949685534591103</v>
       </c>
       <c r="J61" s="2">
-        <v>0.51077414205905802</v>
+        <v>0.42004264392323998</v>
       </c>
       <c r="K61" s="2">
-        <v>0.51397365884998303</v>
+        <v>0.35203716940671897</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -1614,22 +1613,22 @@
         <v>7</v>
       </c>
       <c r="F62" s="2">
-        <v>0.83755528749497299</v>
+        <v>0.85524728588661003</v>
       </c>
       <c r="G62" s="2">
-        <v>0.587096774193548</v>
+        <v>0.554838709677419</v>
       </c>
       <c r="H62" s="2">
-        <v>0.92072844134975895</v>
+        <v>0.95500803427959202</v>
       </c>
       <c r="I62" s="2">
-        <v>0.7109375</v>
+        <v>0.80373831775700899</v>
       </c>
       <c r="J62" s="2">
-        <v>0.64310954063604198</v>
+        <v>0.65648854961832004</v>
       </c>
       <c r="K62" s="2">
-        <v>0.60828877005347504</v>
+        <v>0.59147180192572202</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -1640,22 +1639,22 @@
         <v>8</v>
       </c>
       <c r="F63" s="2">
-        <v>0.60273421793325199</v>
+        <v>0.58423803779654204</v>
       </c>
       <c r="G63" s="2">
-        <v>0.43589743589743501</v>
+        <v>0.48397435897435898</v>
       </c>
       <c r="H63" s="2">
-        <v>0.65861513687600604</v>
+        <v>0.61782071926999405</v>
       </c>
       <c r="I63" s="2">
-        <v>0.29955947136563799</v>
+        <v>0.29783037475345098</v>
       </c>
       <c r="J63" s="2">
-        <v>0.35509138381201</v>
+        <v>0.36874236874236799</v>
       </c>
       <c r="K63" s="2">
-        <v>0.39952996474735603</v>
+        <v>0.43019943019943002</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add task#3; comment on task#4
</commit_message>
<xml_diff>
--- a/A6worksheetV2.xlsx
+++ b/A6worksheetV2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengbo/PycharmProjects/DSTM543-a6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpluskira/studyabroad/Rice/DataSci/A6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEDD54C-BF43-AA42-8A15-65EA14220F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191938D4-1530-5D44-BA1E-8E6B15FDF72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1140" yWindow="460" windowWidth="19700" windowHeight="16560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="27540" windowHeight="15900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="66">
   <si>
     <t>Confusion matrix</t>
   </si>
@@ -158,10 +158,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Bo made an improvement in this part</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> Pokai wrote the model coding part and Bo wrote the metric coding part</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -256,6 +252,12 @@
   <si>
     <t>The F1 and F2 in all the category in task4 model is better than task2 model.</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bo made an improvement in this part; Pokai helped with coding</t>
+  </si>
+  <si>
+    <t>For this, I believe we have to go through Adagrad first since Adadelta is actually an extension of Adagrad. Adadelta, if compared with GD, essentially associates learning rates' change with features' frequencies. That is, Adadelta would update with larger learning rate for parameters associated with infrequent features; on the other hand, it would update with smaller learning rate for those associated with frequent features. And thus, this algorithm might be more suitable when data sparseness increases. If one considers the size of training data being provided (2487) and the number of pixels for each image on three channels (320 X 240 X 3), one would tend to conjecture that there would be some data sparseness issues in this training task. Adadelta is a variant of Adagrad that essentially imposes a regularization coefficient in searching of the parameters.</t>
   </si>
 </sst>
 </file>
@@ -266,7 +268,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -274,13 +276,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -288,7 +290,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -368,7 +370,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -648,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="125" zoomScaleNormal="86" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="86" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,7 +677,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -809,7 +811,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
@@ -1031,7 +1033,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1042,7 +1044,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1178,7 +1180,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F30" s="7">
         <v>70</v>
@@ -1401,10 +1403,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -1415,7 +1417,7 @@
         <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1426,7 +1428,7 @@
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -1434,10 +1436,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
         <v>51</v>
-      </c>
-      <c r="C42" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -1448,7 +1450,7 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -1467,7 +1469,7 @@
         <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -1478,7 +1480,7 @@
         <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -1488,6 +1490,9 @@
       <c r="B47" s="11" t="s">
         <v>30</v>
       </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
@@ -1496,6 +1501,9 @@
       <c r="B48" s="11" t="s">
         <v>31</v>
       </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
@@ -1611,7 +1619,7 @@
         <v>4</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F55" s="7">
         <v>85</v>
@@ -1838,7 +1846,7 @@
         <v>22</v>
       </c>
       <c r="C64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
@@ -1849,7 +1857,7 @@
         <v>23</v>
       </c>
       <c r="C65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -1860,7 +1868,7 @@
         <v>27</v>
       </c>
       <c r="C66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
@@ -1871,7 +1879,7 @@
         <v>23</v>
       </c>
       <c r="C67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -1879,10 +1887,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C68" t="s">
         <v>54</v>
-      </c>
-      <c r="C68" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -1898,10 +1906,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C70" t="s">
         <v>44</v>
-      </c>
-      <c r="C70" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
@@ -1912,7 +1920,7 @@
         <v>34</v>
       </c>
       <c r="C71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -1923,7 +1931,7 @@
         <v>35</v>
       </c>
       <c r="C72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -1934,7 +1942,7 @@
         <v>36</v>
       </c>
       <c r="C73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -2214,7 +2222,7 @@
         <v>86</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F87" s="2">
         <v>0.92802573381584197</v>
@@ -2269,7 +2277,7 @@
         <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
@@ -2280,7 +2288,7 @@
         <v>23</v>
       </c>
       <c r="C90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -2291,7 +2299,7 @@
         <v>27</v>
       </c>
       <c r="C91" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -2302,7 +2310,7 @@
         <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -2313,7 +2321,7 @@
         <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update imag; task3 data; excel
</commit_message>
<xml_diff>
--- a/A6worksheetV2.xlsx
+++ b/A6worksheetV2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpluskira/studyabroad/Rice/DataSci/A6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191938D4-1530-5D44-BA1E-8E6B15FDF72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E05882B-D65B-C641-8F75-40C7FCB49C0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="27540" windowHeight="15900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,10 +190,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>The accuarcy of Monocyte is 620 / 620 = 1,  while others are 0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>The accuarcy of Monocyte is 454 / 620 = 0.73,  while others are 237 / 623 = 0.38 , 292 / 620 =, 270 / 624 = 0.43</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -222,10 +218,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>The accuarcy of Monocyte is 344 / 620 = 0.55,  while others are 270 / 623 = 0.43 , 197 / 620 = 0.32, 302 / 624 = 0.48</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>We change the optimizer to from Adam to Adadelta</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -258,6 +250,12 @@
   </si>
   <si>
     <t>For this, I believe we have to go through Adagrad first since Adadelta is actually an extension of Adagrad. Adadelta, if compared with GD, essentially associates learning rates' change with features' frequencies. That is, Adadelta would update with larger learning rate for parameters associated with infrequent features; on the other hand, it would update with smaller learning rate for those associated with frequent features. And thus, this algorithm might be more suitable when data sparseness increases. If one considers the size of training data being provided (2487) and the number of pixels for each image on three channels (320 X 240 X 3), one would tend to conjecture that there would be some data sparseness issues in this training task. Adadelta is a variant of Adagrad that essentially imposes a regularization coefficient in searching of the parameters.</t>
+  </si>
+  <si>
+    <t>The accuarcy of Monocyte is 233 / 620 = 0.38,  while others are 312 / 623 = 0.5 , 437 / 620 = 0.7 , 274 / 624 = 0.44</t>
+  </si>
+  <si>
+    <t>The accuarcy of Eosinophil is 623 / 623 = 1,  while others are 0</t>
   </si>
 </sst>
 </file>
@@ -340,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -368,6 +366,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="86" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="125" zoomScaleNormal="86" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,7 +706,7 @@
         <v>21</v>
       </c>
       <c r="C5">
-        <v>0.24629999999999999</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -718,7 +717,7 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>23.55</v>
+        <v>22.35</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -764,13 +763,13 @@
         <v>5</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>623</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
       </c>
       <c r="H9" s="2">
-        <v>623</v>
+        <v>0</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
@@ -788,13 +787,13 @@
         <v>6</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>620</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>620</v>
+        <v>0</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -813,14 +812,14 @@
       <c r="E11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="2">
-        <v>0</v>
+      <c r="F11" s="7">
+        <v>620</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
       </c>
-      <c r="H11" s="7">
-        <v>620</v>
+      <c r="H11" s="2">
+        <v>0</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -838,13 +837,13 @@
         <v>8</v>
       </c>
       <c r="F12" s="2">
-        <v>0</v>
+        <v>624</v>
       </c>
       <c r="G12" s="2">
         <v>0</v>
       </c>
       <c r="H12" s="2">
-        <v>624</v>
+        <v>0</v>
       </c>
       <c r="I12" s="2">
         <v>0</v>
@@ -862,14 +861,14 @@
         <v>9</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <f>F9 + F10 + F11 + F12</f>
+        <v>2487</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
       </c>
       <c r="H13" s="2">
-        <f>H9 + H10 + H11 + H12</f>
-        <v>2487</v>
+        <v>0</v>
       </c>
       <c r="I13" s="2">
         <v>0</v>
@@ -928,23 +927,23 @@
       <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F16">
-        <v>0.74949738640932795</v>
-      </c>
-      <c r="G16">
+      <c r="F16" s="2">
+        <v>0.250502613590671</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
         <v>0</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J16" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" t="s">
-        <v>37</v>
+      <c r="I16" s="2">
+        <v>0.250502613590671</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.40064308681672001</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.62562763607149996</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -954,22 +953,22 @@
       <c r="E17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>0.75070365902694003</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>0</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="2">
         <v>1</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -980,23 +979,23 @@
       <c r="E18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F18">
-        <v>0.249296340973059</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="2">
+        <v>0.75070365902694003</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
         <v>1</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0.249296340973059</v>
-      </c>
-      <c r="J18">
-        <v>0.39909880914064999</v>
-      </c>
-      <c r="K18">
-        <v>0.62411918663176902</v>
+      <c r="I18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1006,22 +1005,22 @@
       <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F19">
-        <v>0.74909529553679099</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="2">
+        <v>0.75070365902694003</v>
+      </c>
+      <c r="G19" s="2">
         <v>0</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="2">
         <v>1</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1032,8 +1031,8 @@
       <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
-        <v>47</v>
+      <c r="C20" s="13" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1044,7 +1043,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1417,7 +1416,7 @@
         <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1436,10 +1435,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" t="s">
         <v>50</v>
-      </c>
-      <c r="C42" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -1450,7 +1449,7 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -1469,7 +1468,7 @@
         <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -1480,7 +1479,7 @@
         <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -1491,7 +1490,7 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -1502,7 +1501,7 @@
         <v>31</v>
       </c>
       <c r="C48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -1513,7 +1512,7 @@
         <v>21</v>
       </c>
       <c r="C49">
-        <v>0.83</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -1524,7 +1523,7 @@
         <v>18</v>
       </c>
       <c r="C50">
-        <v>26.61</v>
+        <v>26.97</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
@@ -1569,17 +1568,17 @@
       <c r="E53" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F53" s="2">
-        <v>270</v>
-      </c>
-      <c r="G53" s="2">
-        <v>62</v>
-      </c>
-      <c r="H53" s="2">
-        <v>40</v>
-      </c>
-      <c r="I53" s="2">
-        <v>251</v>
+      <c r="F53">
+        <v>233</v>
+      </c>
+      <c r="G53">
+        <v>49</v>
+      </c>
+      <c r="H53">
+        <v>32</v>
+      </c>
+      <c r="I53">
+        <v>309</v>
       </c>
       <c r="J53" s="2">
         <f>SUM(F53:I53)</f>
@@ -1594,20 +1593,20 @@
       <c r="E54" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F54" s="2">
-        <v>130</v>
-      </c>
-      <c r="G54" s="2">
-        <v>197</v>
-      </c>
-      <c r="H54" s="2">
-        <v>15</v>
-      </c>
-      <c r="I54" s="2">
-        <v>278</v>
+      <c r="F54">
+        <v>95</v>
+      </c>
+      <c r="G54">
+        <v>312</v>
+      </c>
+      <c r="H54">
+        <v>26</v>
+      </c>
+      <c r="I54">
+        <v>187</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" ref="J54:J56" si="2">SUM(F54:I54)</f>
+        <f>SUM(F54:I54)</f>
         <v>620</v>
       </c>
     </row>
@@ -1621,20 +1620,20 @@
       <c r="E55" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F55" s="7">
-        <v>85</v>
-      </c>
-      <c r="G55" s="2">
-        <v>8</v>
-      </c>
-      <c r="H55" s="2">
-        <v>344</v>
-      </c>
-      <c r="I55" s="2">
-        <v>183</v>
+      <c r="F55">
+        <v>58</v>
+      </c>
+      <c r="G55">
+        <v>11</v>
+      </c>
+      <c r="H55">
+        <v>437</v>
+      </c>
+      <c r="I55">
+        <v>114</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" si="2"/>
+        <f>SUM(F55:I55)</f>
         <v>620</v>
       </c>
     </row>
@@ -1646,20 +1645,20 @@
       <c r="E56" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F56" s="2">
-        <v>242</v>
-      </c>
-      <c r="G56" s="2">
-        <v>51</v>
-      </c>
-      <c r="H56" s="2">
-        <v>29</v>
-      </c>
-      <c r="I56" s="2">
-        <v>302</v>
+      <c r="F56">
+        <v>229</v>
+      </c>
+      <c r="G56">
+        <v>65</v>
+      </c>
+      <c r="H56">
+        <v>56</v>
+      </c>
+      <c r="I56">
+        <v>274</v>
       </c>
       <c r="J56" s="2">
-        <f t="shared" si="2"/>
+        <f>SUM(F56:I56)</f>
         <v>624</v>
       </c>
     </row>
@@ -1673,19 +1672,19 @@
       </c>
       <c r="F57" s="2">
         <f>SUM(F53:F56)</f>
-        <v>727</v>
+        <v>615</v>
       </c>
       <c r="G57" s="2">
-        <f t="shared" ref="G57:I57" si="3">SUM(G53:G56)</f>
-        <v>318</v>
+        <f>SUM(G53:G56)</f>
+        <v>437</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" si="3"/>
-        <v>428</v>
+        <f>SUM(H53:H56)</f>
+        <v>551</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" si="3"/>
-        <v>1014</v>
+        <f>SUM(I53:I56)</f>
+        <v>884</v>
       </c>
       <c r="J57" s="2">
         <f>J53 + J54 + J55 + J56</f>
@@ -1741,23 +1740,23 @@
       <c r="E60" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="2">
-        <v>0.67430639324487296</v>
-      </c>
-      <c r="G60" s="2">
-        <v>0.43338683788121901</v>
-      </c>
-      <c r="H60" s="2">
-        <v>0.75482832618025697</v>
-      </c>
-      <c r="I60" s="2">
-        <v>0.371389270976616</v>
-      </c>
-      <c r="J60" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="K60" s="2">
-        <v>0.41938490214352198</v>
+      <c r="F60">
+        <v>0.68958584640128595</v>
+      </c>
+      <c r="G60">
+        <v>0.37399678972712602</v>
+      </c>
+      <c r="H60">
+        <v>0.79506437768240301</v>
+      </c>
+      <c r="I60">
+        <v>0.378861788617886</v>
+      </c>
+      <c r="J60">
+        <v>0.37641357027463601</v>
+      </c>
+      <c r="K60">
+        <v>0.37495976826520699</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -1767,23 +1766,23 @@
       <c r="E61" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F61" s="2">
-        <v>0.78126256533976601</v>
-      </c>
-      <c r="G61" s="2">
-        <v>0.31774193548387097</v>
-      </c>
-      <c r="H61" s="2">
-        <v>0.93519014461703198</v>
-      </c>
-      <c r="I61" s="2">
-        <v>0.61949685534591103</v>
-      </c>
-      <c r="J61" s="2">
-        <v>0.42004264392323998</v>
-      </c>
-      <c r="K61" s="2">
-        <v>0.35203716940671897</v>
+      <c r="F61">
+        <v>0.82589465219139502</v>
+      </c>
+      <c r="G61">
+        <v>0.50322580645161197</v>
+      </c>
+      <c r="H61">
+        <v>0.93304767005891798</v>
+      </c>
+      <c r="I61">
+        <v>0.71395881006864903</v>
+      </c>
+      <c r="J61">
+        <v>0.59035004730368901</v>
+      </c>
+      <c r="K61">
+        <v>0.53479602331162102</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -1793,23 +1792,23 @@
       <c r="E62" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="2">
-        <v>0.85524728588661003</v>
-      </c>
-      <c r="G62" s="2">
-        <v>0.554838709677419</v>
-      </c>
-      <c r="H62" s="2">
-        <v>0.95500803427959202</v>
-      </c>
-      <c r="I62" s="2">
-        <v>0.80373831775700899</v>
-      </c>
-      <c r="J62" s="2">
-        <v>0.65648854961832004</v>
-      </c>
-      <c r="K62" s="2">
-        <v>0.59147180192572202</v>
+      <c r="F62">
+        <v>0.88057901085645296</v>
+      </c>
+      <c r="G62">
+        <v>0.70483870967741902</v>
+      </c>
+      <c r="H62">
+        <v>0.93893947509373299</v>
+      </c>
+      <c r="I62">
+        <v>0.79310344827586199</v>
+      </c>
+      <c r="J62">
+        <v>0.746370623398804</v>
+      </c>
+      <c r="K62">
+        <v>0.72088419663477399</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
@@ -1819,23 +1818,23 @@
       <c r="E63" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="2">
-        <v>0.58423803779654204</v>
-      </c>
-      <c r="G63" s="2">
-        <v>0.48397435897435898</v>
-      </c>
-      <c r="H63" s="2">
-        <v>0.61782071926999405</v>
-      </c>
-      <c r="I63" s="2">
-        <v>0.29783037475345098</v>
-      </c>
-      <c r="J63" s="2">
-        <v>0.36874236874236799</v>
-      </c>
-      <c r="K63" s="2">
-        <v>0.43019943019943002</v>
+      <c r="F63">
+        <v>0.61399276236429401</v>
+      </c>
+      <c r="G63">
+        <v>0.43910256410256399</v>
+      </c>
+      <c r="H63">
+        <v>0.67257112184648404</v>
+      </c>
+      <c r="I63">
+        <v>0.30995475113122101</v>
+      </c>
+      <c r="J63">
+        <v>0.36339522546419101</v>
+      </c>
+      <c r="K63">
+        <v>0.40532544378698199</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -1857,7 +1856,7 @@
         <v>23</v>
       </c>
       <c r="C65" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
@@ -1879,7 +1878,7 @@
         <v>23</v>
       </c>
       <c r="C67" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -1887,10 +1886,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" t="s">
         <v>53</v>
-      </c>
-      <c r="C68" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -1920,7 +1919,7 @@
         <v>34</v>
       </c>
       <c r="C71" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
@@ -1931,7 +1930,7 @@
         <v>35</v>
       </c>
       <c r="C72" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -1942,7 +1941,7 @@
         <v>36</v>
       </c>
       <c r="C73" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
@@ -2288,7 +2287,7 @@
         <v>23</v>
       </c>
       <c r="C90" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -2310,7 +2309,7 @@
         <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -2321,7 +2320,7 @@
         <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>